<commit_message>
removed some sort of invisible character
</commit_message>
<xml_diff>
--- a/data/xlsx/2019-22.xlsx
+++ b/data/xlsx/2019-22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m29605/Documents/github/broomball/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E49C3294-FB46-934F-B0E3-D5073AA73030}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DEAA6FE-EFB6-1D42-81CA-B6EC57451217}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="1" xr2:uid="{3D9C33C8-65AB-974C-BB77-375D6032BA6B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{3D9C33C8-65AB-974C-BB77-375D6032BA6B}"/>
   </bookViews>
   <sheets>
     <sheet name="team" sheetId="4" r:id="rId1"/>
@@ -365,9 +365,6 @@
     <t>Fighting Eeyores</t>
   </si>
   <si>
-    <t>The Suspencer is Killing Me</t>
-  </si>
-  <si>
     <t>Sorcerer's Apparatus</t>
   </si>
   <si>
@@ -702,6 +699,9 @@
   </si>
   <si>
     <t>Meredith Henkleman</t>
+  </si>
+  <si>
+    <t>The Suspencer is Killing Me</t>
   </si>
 </sst>
 </file>
@@ -1086,7 +1086,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F89CCCB8-BB0F-4490-AE5B-B361C4570FB8}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1106,7 +1108,7 @@
     </row>
     <row r="2" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -1117,7 +1119,7 @@
     </row>
     <row r="3" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>105</v>
+        <v>217</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
@@ -1150,13 +1152,13 @@
     </row>
     <row r="6" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1177,24 +1179,24 @@
   <sheetData>
     <row r="1" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>3</v>
@@ -1203,10 +1205,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -1238,7 +1240,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>72</v>
@@ -1278,7 +1280,7 @@
         <v>59</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>60</v>
@@ -1296,10 +1298,10 @@
         <v>83</v>
       </c>
       <c r="K8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -1313,7 +1315,7 @@
         <v>75</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>11</v>
@@ -1325,13 +1327,13 @@
         <v>75</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -1345,13 +1347,13 @@
         <v>75</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>8</v>
@@ -1363,13 +1365,13 @@
         <v>75</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -1383,7 +1385,7 @@
         <v>79</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>11</v>
@@ -1401,13 +1403,13 @@
         <v>75</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -1421,16 +1423,16 @@
         <v>59</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E13" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -1441,16 +1443,16 @@
         <v>75</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F14" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>164</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -1461,16 +1463,16 @@
         <v>79</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>34</v>
@@ -1496,24 +1498,24 @@
   <sheetData>
     <row r="1" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>9</v>
@@ -1522,10 +1524,10 @@
         <v>3</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -1557,10 +1559,10 @@
         <v>9</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>34</v>
@@ -1597,7 +1599,7 @@
         <v>59</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>60</v>
@@ -1615,10 +1617,10 @@
         <v>83</v>
       </c>
       <c r="K8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -1632,7 +1634,7 @@
         <v>75</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>10</v>
@@ -1644,13 +1646,13 @@
         <v>75</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -1664,13 +1666,13 @@
         <v>75</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>34</v>
@@ -1679,13 +1681,13 @@
         <v>75</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -1711,13 +1713,13 @@
         <v>75</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -1731,7 +1733,7 @@
         <v>75</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>10</v>
@@ -1740,7 +1742,7 @@
         <v>31</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>34</v>
@@ -1749,13 +1751,13 @@
         <v>75</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -1769,7 +1771,7 @@
         <v>79</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>10</v>
@@ -1781,13 +1783,13 @@
         <v>75</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -1813,13 +1815,13 @@
         <v>75</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -1833,16 +1835,16 @@
         <v>79</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>34</v>
@@ -1851,13 +1853,13 @@
         <v>75</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -1877,7 +1879,7 @@
         <v>67</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>92</v>
@@ -1903,10 +1905,10 @@
         <v>79</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>91</v>
@@ -1918,7 +1920,7 @@
         <v>56</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1940,24 +1942,24 @@
   <sheetData>
     <row r="1" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>5</v>
@@ -1966,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -2037,7 +2039,7 @@
         <v>59</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>60</v>
@@ -2055,10 +2057,10 @@
         <v>83</v>
       </c>
       <c r="K8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -2072,7 +2074,7 @@
         <v>75</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>36</v>
@@ -2090,13 +2092,13 @@
         <v>75</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -2125,13 +2127,13 @@
         <v>75</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -2160,13 +2162,13 @@
         <v>75</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -2180,7 +2182,7 @@
         <v>79</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>26</v>
@@ -2198,13 +2200,13 @@
         <v>75</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -2230,13 +2232,13 @@
         <v>75</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2257,24 +2259,24 @@
   <sheetData>
     <row r="1" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>9</v>
@@ -2283,10 +2285,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -2314,7 +2316,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>95</v>
@@ -2334,7 +2336,7 @@
         <v>95</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>56</v>
@@ -2354,7 +2356,7 @@
         <v>59</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>60</v>
@@ -2372,10 +2374,10 @@
         <v>83</v>
       </c>
       <c r="K8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -2389,13 +2391,13 @@
         <v>75</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>41</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>6</v>
@@ -2404,13 +2406,13 @@
         <v>75</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -2424,7 +2426,7 @@
         <v>75</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>4</v>
@@ -2439,13 +2441,13 @@
         <v>75</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -2459,7 +2461,7 @@
         <v>79</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>10</v>
@@ -2474,13 +2476,13 @@
         <v>75</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -2494,10 +2496,10 @@
         <v>79</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>6</v>
@@ -2506,13 +2508,13 @@
         <v>75</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -2526,7 +2528,7 @@
         <v>79</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>16</v>
@@ -2544,13 +2546,13 @@
         <v>75</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -2564,7 +2566,7 @@
         <v>79</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>30</v>
@@ -2582,13 +2584,13 @@
         <v>75</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -2608,7 +2610,7 @@
         <v>67</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>92</v>
@@ -2634,7 +2636,7 @@
         <v>75</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>10</v>
@@ -2652,7 +2654,7 @@
         <v>56</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -2666,7 +2668,7 @@
         <v>79</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>4</v>
@@ -2681,7 +2683,7 @@
         <v>6</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2703,24 +2705,24 @@
   <sheetData>
     <row r="1" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
@@ -2729,10 +2731,10 @@
         <v>3</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -2760,7 +2762,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>94</v>
@@ -2780,7 +2782,7 @@
         <v>94</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>56</v>
@@ -2800,7 +2802,7 @@
         <v>59</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>60</v>
@@ -2818,10 +2820,10 @@
         <v>83</v>
       </c>
       <c r="K8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -2835,7 +2837,7 @@
         <v>75</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>29</v>
@@ -2844,7 +2846,7 @@
         <v>16</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>56</v>
@@ -2853,13 +2855,13 @@
         <v>75</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -2873,7 +2875,7 @@
         <v>79</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>24</v>
@@ -2888,13 +2890,13 @@
         <v>75</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -2908,7 +2910,7 @@
         <v>79</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>16</v>
@@ -2923,13 +2925,13 @@
         <v>75</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -2943,10 +2945,10 @@
         <v>79</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>24</v>
@@ -2961,13 +2963,13 @@
         <v>75</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -2987,7 +2989,7 @@
         <v>67</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>92</v>
@@ -3013,7 +3015,7 @@
         <v>79</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>24</v>
@@ -3028,7 +3030,7 @@
         <v>56</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -3049,24 +3051,24 @@
   <sheetData>
     <row r="1" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>5</v>
@@ -3075,10 +3077,10 @@
         <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -3106,7 +3108,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>72</v>
@@ -3146,7 +3148,7 @@
         <v>59</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>60</v>
@@ -3164,10 +3166,10 @@
         <v>83</v>
       </c>
       <c r="K8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -3181,7 +3183,7 @@
         <v>75</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>24</v>
@@ -3196,13 +3198,13 @@
         <v>75</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -3216,7 +3218,7 @@
         <v>75</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>36</v>
@@ -3234,13 +3236,13 @@
         <v>75</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -3254,7 +3256,7 @@
         <v>75</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>21</v>
@@ -3269,13 +3271,13 @@
         <v>75</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -3289,7 +3291,7 @@
         <v>75</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>20</v>
@@ -3307,13 +3309,13 @@
         <v>75</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -3327,7 +3329,7 @@
         <v>79</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>49</v>
@@ -3342,13 +3344,13 @@
         <v>75</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -3368,7 +3370,7 @@
         <v>67</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>92</v>
@@ -3394,7 +3396,7 @@
         <v>75</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>12</v>
@@ -3409,7 +3411,7 @@
         <v>6</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -3430,24 +3432,24 @@
   <sheetData>
     <row r="1" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>9</v>
@@ -3456,10 +3458,10 @@
         <v>3</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -3487,10 +3489,10 @@
         <v>9</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>8</v>
@@ -3527,7 +3529,7 @@
         <v>59</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>60</v>
@@ -3545,10 +3547,10 @@
         <v>83</v>
       </c>
       <c r="K8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -3562,7 +3564,7 @@
         <v>75</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>10</v>
@@ -3577,13 +3579,13 @@
         <v>75</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -3597,7 +3599,7 @@
         <v>75</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>29</v>
@@ -3612,13 +3614,13 @@
         <v>75</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -3644,16 +3646,16 @@
         <v>8</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -3676,16 +3678,16 @@
         <v>6</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -3699,22 +3701,22 @@
         <v>79</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>8</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -3734,16 +3736,16 @@
         <v>8</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -3766,16 +3768,16 @@
         <v>6</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -3798,16 +3800,16 @@
         <v>6</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -3830,16 +3832,16 @@
         <v>8</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -3859,7 +3861,7 @@
         <v>67</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>92</v>
@@ -3882,7 +3884,7 @@
         <v>3</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>91</v>
@@ -3935,24 +3937,24 @@
   <sheetData>
     <row r="1" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>9</v>
@@ -3961,10 +3963,10 @@
         <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4001,7 +4003,7 @@
         <v>94</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>56</v>
@@ -4015,7 +4017,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>72</v>
@@ -4041,7 +4043,7 @@
         <v>59</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>60</v>
@@ -4059,10 +4061,10 @@
         <v>83</v>
       </c>
       <c r="K8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4076,7 +4078,7 @@
         <v>75</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>22</v>
@@ -4091,13 +4093,13 @@
         <v>75</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4111,10 +4113,10 @@
         <v>79</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>74</v>
@@ -4123,13 +4125,13 @@
         <v>75</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4158,13 +4160,13 @@
         <v>75</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4178,7 +4180,7 @@
         <v>79</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>10</v>
@@ -4196,13 +4198,13 @@
         <v>75</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4216,10 +4218,10 @@
         <v>98</v>
       </c>
       <c r="D13" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>207</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>208</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>74</v>
@@ -4228,13 +4230,13 @@
         <v>75</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4254,7 +4256,7 @@
         <v>67</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>92</v>
@@ -4277,7 +4279,7 @@
         <v>9</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>85</v>
@@ -4289,7 +4291,7 @@
         <v>74</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -4312,24 +4314,24 @@
   <sheetData>
     <row r="1" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>3</v>
@@ -4338,10 +4340,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4358,7 +4360,7 @@
         <v>59</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>60</v>
@@ -4376,10 +4378,10 @@
         <v>83</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4393,7 +4395,7 @@
         <v>75</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>39</v>
@@ -4402,7 +4404,7 @@
         <v>29</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>55</v>
@@ -4411,13 +4413,13 @@
         <v>75</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4431,7 +4433,7 @@
         <v>75</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>27</v>
@@ -4446,13 +4448,13 @@
         <v>75</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4481,13 +4483,13 @@
         <v>75</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4501,7 +4503,7 @@
         <v>75</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>56</v>
@@ -4516,13 +4518,13 @@
         <v>75</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4536,7 +4538,7 @@
         <v>79</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>20</v>
@@ -4551,13 +4553,13 @@
         <v>75</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4571,7 +4573,7 @@
         <v>79</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>6</v>
@@ -4586,13 +4588,13 @@
         <v>75</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4606,7 +4608,7 @@
         <v>79</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>6</v>
@@ -4618,16 +4620,16 @@
         <v>34</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>75</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4647,7 +4649,7 @@
         <v>67</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>92</v>
@@ -4673,7 +4675,7 @@
         <v>75</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>31</v>
@@ -4688,7 +4690,7 @@
         <v>34</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4702,7 +4704,7 @@
         <v>79</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>31</v>
@@ -4729,7 +4731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8A4E20C-A8D6-784F-B3B9-729D70553C62}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -4752,7 +4754,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4769,7 +4771,7 @@
         <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4786,7 +4788,7 @@
         <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4803,7 +4805,7 @@
         <v>22</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4820,7 +4822,7 @@
         <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4834,10 +4836,10 @@
         <v>28</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4854,7 +4856,7 @@
         <v>31</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4871,7 +4873,7 @@
         <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4896,7 +4898,7 @@
         <v>39</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>40</v>
@@ -4916,7 +4918,7 @@
         <v>44</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4963,24 +4965,24 @@
   <sheetData>
     <row r="1" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
@@ -4992,7 +4994,7 @@
         <v>52</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -5060,7 +5062,7 @@
         <v>59</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>60</v>
@@ -5078,10 +5080,10 @@
         <v>83</v>
       </c>
       <c r="K8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -5113,13 +5115,13 @@
         <v>75</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -5148,13 +5150,13 @@
         <v>75</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -5183,13 +5185,13 @@
         <v>75</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -5209,7 +5211,7 @@
         <v>67</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>92</v>
@@ -5250,7 +5252,7 @@
         <v>56</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -5271,24 +5273,24 @@
   <sheetData>
     <row r="1" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -5300,7 +5302,7 @@
         <v>52</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -5368,7 +5370,7 @@
         <v>59</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>60</v>
@@ -5386,10 +5388,10 @@
         <v>83</v>
       </c>
       <c r="K8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -5421,13 +5423,13 @@
         <v>75</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -5456,13 +5458,13 @@
         <v>75</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -5494,13 +5496,13 @@
         <v>75</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -5526,13 +5528,13 @@
         <v>75</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -5561,13 +5563,13 @@
         <v>75</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -5596,10 +5598,10 @@
         <v>75</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -5628,16 +5630,16 @@
         <v>56</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -5657,7 +5659,7 @@
         <v>67</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>92</v>
@@ -5698,7 +5700,7 @@
         <v>56</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -5806,24 +5808,24 @@
   <sheetData>
     <row r="1" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
@@ -5835,7 +5837,7 @@
         <v>93</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -5903,7 +5905,7 @@
         <v>59</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>60</v>
@@ -5921,10 +5923,10 @@
         <v>83</v>
       </c>
       <c r="K8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -5953,13 +5955,13 @@
         <v>75</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -5988,10 +5990,10 @@
         <v>75</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>75</v>
@@ -6020,24 +6022,24 @@
   <sheetData>
     <row r="1" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
@@ -6049,7 +6051,7 @@
         <v>93</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -6117,7 +6119,7 @@
         <v>59</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>60</v>
@@ -6135,10 +6137,10 @@
         <v>83</v>
       </c>
       <c r="K8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -6170,13 +6172,13 @@
         <v>75</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -6208,13 +6210,13 @@
         <v>75</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -6240,13 +6242,13 @@
         <v>75</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -6275,13 +6277,13 @@
         <v>75</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -6301,7 +6303,7 @@
         <v>67</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>92</v>
@@ -6339,7 +6341,7 @@
         <v>55</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -6365,7 +6367,7 @@
         <v>6</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -6388,24 +6390,24 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>5</v>
@@ -6414,10 +6416,10 @@
         <v>9</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -6445,7 +6447,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>98</v>
@@ -6485,7 +6487,7 @@
         <v>59</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>60</v>
@@ -6503,10 +6505,10 @@
         <v>83</v>
       </c>
       <c r="K8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -6520,7 +6522,7 @@
         <v>75</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>41</v>
@@ -6529,7 +6531,7 @@
         <v>39</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>55</v>
@@ -6538,13 +6540,13 @@
         <v>75</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -6558,13 +6560,13 @@
         <v>75</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>47</v>
@@ -6576,13 +6578,13 @@
         <v>75</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -6596,7 +6598,7 @@
         <v>75</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>12</v>
@@ -6608,13 +6610,13 @@
         <v>75</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -6628,7 +6630,7 @@
         <v>79</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>11</v>
@@ -6640,13 +6642,13 @@
         <v>75</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -6660,7 +6662,7 @@
         <v>79</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>8</v>
@@ -6678,13 +6680,13 @@
         <v>75</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -6698,13 +6700,13 @@
         <v>79</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>55</v>
@@ -6713,13 +6715,13 @@
         <v>75</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:12" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6740,7 +6742,7 @@
         <v>67</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>92</v>
@@ -6766,7 +6768,7 @@
         <v>75</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>8</v>
@@ -6781,7 +6783,7 @@
         <v>74</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -6795,7 +6797,7 @@
         <v>75</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>47</v>
@@ -6810,7 +6812,7 @@
         <v>74</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -6824,7 +6826,7 @@
         <v>79</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>39</v>
@@ -6839,7 +6841,7 @@
         <v>74</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -6860,19 +6862,19 @@
   <sheetData>
     <row r="1" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -6881,7 +6883,7 @@
     </row>
     <row r="2" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>3</v>
@@ -6890,10 +6892,10 @@
         <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -6925,10 +6927,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>34</v>
@@ -6942,7 +6944,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>73</v>
@@ -6965,7 +6967,7 @@
         <v>59</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>60</v>
@@ -6983,10 +6985,10 @@
         <v>83</v>
       </c>
       <c r="K8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -7000,7 +7002,7 @@
         <v>75</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>44</v>
@@ -7012,13 +7014,13 @@
         <v>75</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -7032,7 +7034,7 @@
         <v>75</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>24</v>
@@ -7050,13 +7052,13 @@
         <v>75</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -7070,7 +7072,7 @@
         <v>75</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>37</v>
@@ -7088,13 +7090,13 @@
         <v>75</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -7108,7 +7110,7 @@
         <v>79</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>15</v>
@@ -7123,13 +7125,13 @@
         <v>75</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -7143,7 +7145,7 @@
         <v>79</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>6</v>
@@ -7158,13 +7160,13 @@
         <v>75</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -7178,7 +7180,7 @@
         <v>79</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>11</v>
@@ -7196,13 +7198,13 @@
         <v>75</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -7233,7 +7235,7 @@
         <v>67</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>92</v>
@@ -7274,7 +7276,7 @@
         <v>56</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -7288,16 +7290,16 @@
         <v>59</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E19" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -7308,13 +7310,13 @@
         <v>79</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>56</v>
@@ -7338,24 +7340,24 @@
   <sheetData>
     <row r="1" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>9</v>
@@ -7364,10 +7366,10 @@
         <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -7399,7 +7401,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>98</v>
@@ -7416,10 +7418,10 @@
         <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>55</v>
@@ -7439,7 +7441,7 @@
         <v>59</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>60</v>
@@ -7457,10 +7459,10 @@
         <v>83</v>
       </c>
       <c r="K8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -7474,7 +7476,7 @@
         <v>75</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>49</v>
@@ -7489,13 +7491,13 @@
         <v>75</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -7509,7 +7511,7 @@
         <v>75</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>21</v>
@@ -7521,13 +7523,13 @@
         <v>75</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -7541,7 +7543,7 @@
         <v>75</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>8</v>
@@ -7553,13 +7555,13 @@
         <v>75</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -7573,10 +7575,10 @@
         <v>75</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>20</v>
@@ -7589,13 +7591,13 @@
         <v>75</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -7609,10 +7611,10 @@
         <v>75</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>37</v>
@@ -7624,13 +7626,13 @@
         <v>75</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -7644,7 +7646,7 @@
         <v>75</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>31</v>
@@ -7656,13 +7658,13 @@
         <v>75</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -7676,10 +7678,10 @@
         <v>79</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>34</v>
@@ -7688,13 +7690,13 @@
         <v>75</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -7708,13 +7710,13 @@
         <v>79</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>21</v>
@@ -7726,13 +7728,13 @@
         <v>75</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -7761,13 +7763,13 @@
         <v>75</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -7781,13 +7783,13 @@
         <v>79</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>55</v>
@@ -7796,13 +7798,13 @@
         <v>75</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -7822,7 +7824,7 @@
         <v>67</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>92</v>
@@ -7848,7 +7850,7 @@
         <v>79</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>11</v>
@@ -7863,7 +7865,7 @@
         <v>55</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
using database for season stats...
</commit_message>
<xml_diff>
--- a/data/xlsx/2019-22.xlsx
+++ b/data/xlsx/2019-22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m29605/Documents/github/broomball/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DEAA6FE-EFB6-1D42-81CA-B6EC57451217}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D630EC-3E2C-3546-A67C-D47B7B253642}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{3D9C33C8-65AB-974C-BB77-375D6032BA6B}"/>
   </bookViews>
@@ -1086,9 +1086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F89CCCB8-BB0F-4490-AE5B-B361C4570FB8}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1487,9 +1485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5165660-993F-5F47-B553-82EE84FD6BE8}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1914,7 +1910,7 @@
         <v>91</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>56</v>
@@ -2648,7 +2644,7 @@
         <v>91</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>56</v>
@@ -2677,7 +2673,7 @@
         <v>85</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>6</v>
@@ -3024,7 +3020,7 @@
         <v>91</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>56</v>
@@ -3405,7 +3401,7 @@
         <v>85</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>6</v>
@@ -3890,7 +3886,7 @@
         <v>91</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>8</v>
@@ -3910,7 +3906,7 @@
         <v>18</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>6</v>
@@ -4285,7 +4281,7 @@
         <v>85</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>74</v>
@@ -4303,9 +4299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E743939D-990D-E14D-8A36-65C92ED6237F}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4684,7 +4678,7 @@
         <v>71</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>34</v>
@@ -4713,7 +4707,7 @@
         <v>91</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>34</v>
@@ -4731,9 +4725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8A4E20C-A8D6-784F-B3B9-729D70553C62}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5246,7 +5238,7 @@
         <v>71</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>56</v>
@@ -5694,7 +5686,7 @@
         <v>85</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>56</v>
@@ -5723,7 +5715,7 @@
         <v>85</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>56</v>
@@ -5752,7 +5744,7 @@
         <v>89</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>56</v>
@@ -5781,7 +5773,7 @@
         <v>91</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>74</v>
@@ -6335,7 +6327,7 @@
         <v>91</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>55</v>
@@ -6361,7 +6353,7 @@
         <v>102</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>6</v>
@@ -6379,9 +6371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54D57F14-7291-8047-B4A7-36F1DA33FCAF}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6777,7 +6767,7 @@
         <v>91</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>74</v>
@@ -6806,7 +6796,7 @@
         <v>91</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>74</v>
@@ -6835,7 +6825,7 @@
         <v>91</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>74</v>
@@ -7270,7 +7260,7 @@
         <v>85</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>56</v>
@@ -7859,7 +7849,7 @@
         <v>71</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
using dbAppendTable instead of dbWriteTable, fixed foreign key violations due to mispelling, etc..., also allowing some null values...
</commit_message>
<xml_diff>
--- a/data/xlsx/2019-22.xlsx
+++ b/data/xlsx/2019-22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m29605/Documents/github/broomball/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D630EC-3E2C-3546-A67C-D47B7B253642}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA50CDDF-1142-7946-B245-ACA5E8BD0B9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{3D9C33C8-65AB-974C-BB77-375D6032BA6B}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1980" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1979" uniqueCount="217">
   <si>
     <t>team</t>
   </si>
@@ -515,9 +515,6 @@
     <t>server</t>
   </si>
   <si>
-    <t>Free Agent</t>
-  </si>
-  <si>
     <t>grey</t>
   </si>
   <si>
@@ -551,9 +548,6 @@
     <t>03:15</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Nik Moy</t>
   </si>
   <si>
@@ -702,6 +696,9 @@
   </si>
   <si>
     <t>The Suspencer is Killing Me</t>
+  </si>
+  <si>
+    <t>Free Agent 1</t>
   </si>
 </sst>
 </file>
@@ -1086,7 +1083,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F89CCCB8-BB0F-4490-AE5B-B361C4570FB8}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1117,7 +1116,7 @@
     </row>
     <row r="3" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
@@ -1150,13 +1149,10 @@
     </row>
     <row r="6" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1238,7 +1234,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>72</v>
@@ -1313,7 +1309,7 @@
         <v>75</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>11</v>
@@ -1345,13 +1341,13 @@
         <v>75</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>8</v>
@@ -1383,7 +1379,7 @@
         <v>79</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>11</v>
@@ -1441,16 +1437,16 @@
         <v>75</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F14" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>163</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -1461,10 +1457,10 @@
         <v>79</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>5</v>
@@ -1520,7 +1516,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>136</v>
@@ -1630,7 +1626,7 @@
         <v>75</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>10</v>
@@ -1662,7 +1658,7 @@
         <v>75</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>10</v>
@@ -1729,7 +1725,7 @@
         <v>75</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>10</v>
@@ -1738,7 +1734,7 @@
         <v>31</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>34</v>
@@ -1831,7 +1827,7 @@
         <v>79</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>10</v>
@@ -1840,7 +1836,7 @@
         <v>110</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>34</v>
@@ -1901,7 +1897,7 @@
         <v>79</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>110</v>
@@ -1964,7 +1960,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>136</v>
@@ -2070,7 +2066,7 @@
         <v>75</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>36</v>
@@ -2178,7 +2174,7 @@
         <v>79</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>26</v>
@@ -2281,7 +2277,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>136</v>
@@ -2387,13 +2383,13 @@
         <v>75</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>41</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>6</v>
@@ -2422,7 +2418,7 @@
         <v>75</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>4</v>
@@ -2457,7 +2453,7 @@
         <v>79</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>10</v>
@@ -2492,10 +2488,10 @@
         <v>79</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>6</v>
@@ -2524,7 +2520,7 @@
         <v>79</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>16</v>
@@ -2562,7 +2558,7 @@
         <v>79</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>30</v>
@@ -2632,7 +2628,7 @@
         <v>75</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>10</v>
@@ -2664,7 +2660,7 @@
         <v>79</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>4</v>
@@ -2727,7 +2723,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>136</v>
@@ -2778,7 +2774,7 @@
         <v>94</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>56</v>
@@ -2833,7 +2829,7 @@
         <v>75</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>29</v>
@@ -2842,7 +2838,7 @@
         <v>16</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>56</v>
@@ -2871,7 +2867,7 @@
         <v>79</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>24</v>
@@ -2906,7 +2902,7 @@
         <v>79</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>16</v>
@@ -2941,10 +2937,10 @@
         <v>79</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>24</v>
@@ -3011,7 +3007,7 @@
         <v>79</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>24</v>
@@ -3073,7 +3069,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>136</v>
@@ -3179,7 +3175,7 @@
         <v>75</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>24</v>
@@ -3214,7 +3210,7 @@
         <v>75</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>36</v>
@@ -3252,7 +3248,7 @@
         <v>75</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>21</v>
@@ -3287,7 +3283,7 @@
         <v>75</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>20</v>
@@ -3325,7 +3321,7 @@
         <v>79</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>49</v>
@@ -3392,7 +3388,7 @@
         <v>75</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>12</v>
@@ -3454,7 +3450,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>136</v>
@@ -3485,10 +3481,10 @@
         <v>9</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>8</v>
@@ -3560,7 +3556,7 @@
         <v>75</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>10</v>
@@ -3595,7 +3591,7 @@
         <v>75</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>29</v>
@@ -3880,7 +3876,7 @@
         <v>3</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>91</v>
@@ -3959,7 +3955,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>136</v>
@@ -4074,7 +4070,7 @@
         <v>75</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>22</v>
@@ -4112,7 +4108,7 @@
         <v>111</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>74</v>
@@ -4176,7 +4172,7 @@
         <v>79</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>10</v>
@@ -4214,10 +4210,10 @@
         <v>98</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>74</v>
@@ -4275,7 +4271,7 @@
         <v>9</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>85</v>
@@ -4334,7 +4330,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>136</v>
@@ -4389,7 +4385,7 @@
         <v>75</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>39</v>
@@ -4427,7 +4423,7 @@
         <v>75</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>27</v>
@@ -4497,7 +4493,7 @@
         <v>75</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>56</v>
@@ -4532,7 +4528,7 @@
         <v>79</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>20</v>
@@ -4567,7 +4563,7 @@
         <v>79</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>6</v>
@@ -4669,7 +4665,7 @@
         <v>75</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>31</v>
@@ -4698,7 +4694,7 @@
         <v>79</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>31</v>
@@ -4746,7 +4742,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4763,7 +4759,7 @@
         <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4814,7 +4810,7 @@
         <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4831,7 +4827,7 @@
         <v>110</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4848,7 +4844,7 @@
         <v>31</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4865,7 +4861,7 @@
         <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4890,7 +4886,7 @@
         <v>39</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>40</v>
@@ -4910,7 +4906,7 @@
         <v>44</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -6696,7 +6692,7 @@
         <v>18</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>55</v>
@@ -7604,7 +7600,7 @@
         <v>146</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>37</v>
@@ -7706,7 +7702,7 @@
         <v>37</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>21</v>
@@ -7779,7 +7775,7 @@
         <v>21</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
add season, name fix, code update
</commit_message>
<xml_diff>
--- a/data/xlsx/2019-22.xlsx
+++ b/data/xlsx/2019-22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnanto/GitHub/broomball/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8898CC4F-994C-FB4F-90A7-20CF449947D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F556E3ED-E971-BD41-A6D7-7CB2A2829044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17540" xr2:uid="{3D9C33C8-65AB-974C-BB77-375D6032BA6B}"/>
   </bookViews>
@@ -680,9 +680,6 @@
     <t>02:35</t>
   </si>
   <si>
-    <t>Michelle LaFramboise</t>
-  </si>
-  <si>
     <t>Meredith Henkleman</t>
   </si>
   <si>
@@ -696,6 +693,9 @@
   </si>
   <si>
     <t>Katy Bright</t>
+  </si>
+  <si>
+    <t>Michelle Nudi</t>
   </si>
 </sst>
 </file>
@@ -1081,7 +1081,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1113,7 +1113,7 @@
     </row>
     <row r="3" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
@@ -1146,7 +1146,7 @@
     </row>
     <row r="6" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>153</v>
@@ -1346,7 +1346,7 @@
         <v>197</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>8</v>
@@ -1733,7 +1733,7 @@
         <v>29</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>32</v>
@@ -1835,7 +1835,7 @@
         <v>108</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>32</v>
@@ -4462,7 +4462,7 @@
         <v>37</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>53</v>
@@ -4781,7 +4781,7 @@
     </row>
     <row r="4" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>19</v>
@@ -4810,7 +4810,7 @@
         <v>197</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -4886,7 +4886,7 @@
         <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>38</v>
@@ -4906,7 +4906,7 @@
         <v>42</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -6694,7 +6694,7 @@
         <v>18</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
update stats, fix names...
</commit_message>
<xml_diff>
--- a/data/xlsx/2019-22.xlsx
+++ b/data/xlsx/2019-22.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnanto/GitHub/broomball/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F556E3ED-E971-BD41-A6D7-7CB2A2829044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1262924-03CC-CD4E-85F0-F37487F71A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17540" xr2:uid="{3D9C33C8-65AB-974C-BB77-375D6032BA6B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{3D9C33C8-65AB-974C-BB77-375D6032BA6B}"/>
   </bookViews>
   <sheets>
     <sheet name="team" sheetId="4" r:id="rId1"/>
@@ -782,9 +782,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -822,7 +822,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -928,7 +928,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1070,7 +1070,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1080,7 +1080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F89CCCB8-BB0F-4490-AE5B-B361C4570FB8}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
@@ -4719,16 +4719,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8A4E20C-A8D6-784F-B3B9-729D70553C62}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -4745,7 +4748,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -4762,7 +4765,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -4779,7 +4782,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>214</v>
       </c>
@@ -4796,7 +4799,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -4813,7 +4816,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -4830,7 +4833,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -4847,7 +4850,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -4864,7 +4867,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
@@ -4881,7 +4884,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
@@ -4895,7 +4898,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
@@ -4909,7 +4912,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
@@ -4923,7 +4926,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>46</v>
       </c>

</xml_diff>